<commit_message>
check next cell and change result string to list
</commit_message>
<xml_diff>
--- a/reuslt.xlsx
+++ b/reuslt.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:A2"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -421,10 +421,165 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>예윤</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>재현 서연 태훈</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>예윤</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>재현 예윤 혜지 태훈 한솔 서연</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>재현 서연 태훈</t>
+        </is>
+      </c>
+    </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
           <t>예윤 유진</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>재현 태훈</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>희지 유진</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>병국 재현 예윤 현빈 희지 혜지 태훈 한솔 서연</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>재현 태훈</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>재현 혜지 유진</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>태훈</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>재현 혜지 유진</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>한솔 서연</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>병국 현빈 희지</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>재현 혜지 서연</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>태훈</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>재현 혜지 서연</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>준범 한솔 서연</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>병국 예윤 현빈 희지 유진 한솔</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>재현 혜지 서연 한솔</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>예윤 유진 태훈</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>재현 혜지 한솔 서연</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>예윤 준범 유진 한솔 서연</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>병국 예윤 현빈 희지 유진</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>재현 희지 혜지 서연 한솔</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>예윤 현빈 희지 혜지 유진 태훈</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>병국 재현 희지 혜지 한솔 서연</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>재현 예윤 현빈 희지 혜지 준범 유진 한솔 서연</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>병국 예윤 현빈 희지 혜지 유진 태훈</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
modify SortInNum and make UpateTime function
</commit_message>
<xml_diff>
--- a/reuslt.xlsx
+++ b/reuslt.xlsx
@@ -429,22 +429,22 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>서연 태훈</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>예윤</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>태훈 서연</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>예윤</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>서연 한솔</t>
-        </is>
-      </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>태훈 서연</t>
+          <t>서연 태훈</t>
         </is>
       </c>
     </row>
@@ -461,12 +461,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>유진 희지</t>
+          <t>희지 유진</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>서연 한솔</t>
+          <t>현빈 병국</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -478,7 +478,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>유진 혜지</t>
+          <t>유진 재현</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -488,7 +488,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>유진 혜지</t>
+          <t>유진 재현</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -498,14 +498,14 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>희지 현빈</t>
+          <t>현빈 병국</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>서연 혜지</t>
+          <t>서연 재현</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -515,29 +515,29 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>서연 혜지</t>
+          <t>서연 재현</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>서연 한솔</t>
+          <t>준범 서연</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>한솔 유진</t>
+          <t>현빈 병국</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>한솔 서연</t>
+          <t>서연 한솔</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>태훈 유진</t>
+          <t>태훈 예윤</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -547,39 +547,39 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>서연 한솔</t>
+          <t>준범 서연</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>유진 희지</t>
+          <t>현빈 병국</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>한솔 서연</t>
+          <t>희지 서연</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>태훈 유진</t>
+          <t>현빈 희지</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>서연 한솔</t>
+          <t>병국 희지</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>서연 한솔</t>
+          <t>준범 현빈</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>태훈 유진</t>
+          <t>현빈 병국</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
put person in left list
</commit_message>
<xml_diff>
--- a/reuslt.xlsx
+++ b/reuslt.xlsx
@@ -424,7 +424,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>예윤</t>
+          <t>예윤 병국</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -434,7 +434,7 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>예윤</t>
+          <t>예윤 병국</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
@@ -483,7 +483,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>태훈</t>
+          <t>태훈 현빈</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -510,7 +510,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>태훈</t>
+          <t>태훈 태훈</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">

</xml_diff>

<commit_message>
modify time check but not perfect
</commit_message>
<xml_diff>
--- a/reuslt.xlsx
+++ b/reuslt.xlsx
@@ -439,12 +439,12 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>서연 태훈</t>
+          <t>서연</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>태훈 재현</t>
+          <t>현빈</t>
         </is>
       </c>
     </row>
@@ -466,14 +466,10 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>현빈 서연</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>태훈 재현</t>
-        </is>
-      </c>
+          <t>현빈 병국</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -488,19 +484,15 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>재현 혜지</t>
+          <t>유진 재현</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>한솔 현빈</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>현빈 병국</t>
-        </is>
-      </c>
+          <t>현빈</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -520,14 +512,10 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>준범 한솔</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>현빈 희지</t>
-        </is>
-      </c>
+          <t>준범</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -542,19 +530,15 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>서연 한솔</t>
+          <t>서연 태훈</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>준범 한솔</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>현빈 희지</t>
-        </is>
-      </c>
+          <t>준범</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -574,41 +558,29 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>한솔 준범</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>현빈 태훈</t>
-        </is>
-      </c>
+          <t>준범 현빈</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>한솔 유진</t>
+          <t>한솔 희지</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>한솔 유진</t>
+          <t>한솔 희지</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>준범 한솔</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>한솔 준범</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>한솔 유진</t>
-        </is>
-      </c>
+          <t>준범</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>

<commit_message>
modify update time result_list
</commit_message>
<xml_diff>
--- a/reuslt.xlsx
+++ b/reuslt.xlsx
@@ -439,12 +439,12 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>서연</t>
+          <t>서연 한솔</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>현빈</t>
+          <t>태훈 재현</t>
         </is>
       </c>
     </row>
@@ -456,25 +456,29 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>태훈 서연</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>예윤 희지</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>현빈 태훈</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
           <t>태훈 재현</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>희지 유진</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>현빈 병국</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>유진 재현</t>
+          <t>병국 유진</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -484,20 +488,24 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>유진 재현</t>
+          <t>희지 유진</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>현빈</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr"/>
+          <t>현빈 태훈</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>재현 병국</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>서연 재현</t>
+          <t>유진 서연</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -507,7 +515,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>서연 재현</t>
+          <t>유진 서연</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -515,53 +523,65 @@
           <t>준범</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>병국 희지</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>한솔 서연</t>
+          <t>서연 한솔</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>태훈 유진</t>
+          <t>태훈 예윤</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>서연 태훈</t>
+          <t>서연 한솔</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>준범</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr"/>
+          <t>준범 유진</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>병국</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>한솔 서연</t>
+          <t>서연 한솔</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>희지 현빈</t>
+          <t>예윤 현빈</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>병국 서연</t>
+          <t>서연 한솔</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>준범 현빈</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr"/>
+          <t>준범 희지</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>병국 혜지</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -571,16 +591,24 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>한솔 희지</t>
+          <t>현빈 예윤</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>준범</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
+          <t>준범 유진</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>희지 현빈</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>혜지</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>